<commit_message>
Eliminate RTL Freeze terminology in spreadsheet
</commit_message>
<xml_diff>
--- a/process/OpenHW-Group-IP-Core-RTL-Freeze-Checklist-Templates/OpenHWGroup_TRL5_for_COREV_RTL_IP_Template.xlsx
+++ b/process/OpenHW-Group-IP-Core-RTL-Freeze-Checklist-Templates/OpenHWGroup_TRL5_for_COREV_RTL_IP_Template.xlsx
@@ -25,18 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="149">
-  <si>
-    <t xml:space="preserve">Copyright 2020 by the OpenHW Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Licensed under the Solderpad Hardware License, Version 2.0</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="148">
+  <si>
+    <t xml:space="preserve">Copyright 2020, 2023 by the OpenHW Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licensed under the Solderpad Hardware License, Version 2.1</t>
   </si>
   <si>
     <t xml:space="preserve">Purpose of this Document</t>
   </si>
   <si>
-    <t xml:space="preserve">This document is the Checklist for the “Functional RTL Freeze” criteria for OpenHW Group RTL IP.</t>
+    <t xml:space="preserve">This document is the Checklist for the TRL-5 Release for OpenHW Group RTL IP.</t>
   </si>
   <si>
     <t xml:space="preserve">RTL IP</t>
@@ -45,13 +45,13 @@
     <t xml:space="preserve">For the purposes of this document, RTL IP shall mean designs and associated collateral that can be use to realize a functional design in either an FPGA, ASIC or both.  The RTL IP is captured as synthesizable SystemVerilog.</t>
   </si>
   <si>
-    <t xml:space="preserve">What Does “Functional RTL Freeze” Mean?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RTL that means the Functional RTL Freeze criteria is complete, functionally correct, validated against a specific software toolchain and ready to be used in a commercial-grade product.  The Specification, Design and Verification are complete and self-consistent.  It has been shown to match the design intent as captured in the specification by means of either dynamic or static verification methods (or both).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deliverables: OpenHW provides the following at RTL Freeze:</t>
+    <t xml:space="preserve">What Does “TRL-5” Mean?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTL that meets the TRL-5 criteria is complete, functionally correct, validated against a specific software toolchain and ready to be used in a commercial-grade product.  The Specification, Design and Verification are complete and self-consistent.  It has been shown to match the design intent as captured in the specification by means of either dynamic or static verification methods (or both).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deliverables: OpenHW provides the following at TRL-5:</t>
   </si>
   <si>
     <t xml:space="preserve">- A complete User Manual including implementation guidelines</t>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">A note out Physical Implementations</t>
   </si>
   <si>
-    <t xml:space="preserve">IP that achieves the Functional RTL Freeze milestone is subject to a set of design rules and lint checks.  It may or may not have been synthesized and implemented into a physical gate model.</t>
+    <t xml:space="preserve">IP that achieves the TRL-5 criteria is subject to a set of RTL design rules and lint checks.  It may or may not have been synthesized and implemented into a physical gate model.</t>
   </si>
   <si>
     <t xml:space="preserve">Category</t>
@@ -162,10 +162,7 @@
     <t xml:space="preserve">Version clearly identified</t>
   </si>
   <si>
-    <t xml:space="preserve">The version at this release is clearly identified in GitHub and in the RTL freeze review document.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arjan.bink@silabs.com</t>
+    <t xml:space="preserve">The version at this release is clearly identified in GitHub and in the release review document.</t>
   </si>
   <si>
     <t xml:space="preserve">Coding rules</t>
@@ -216,7 +213,7 @@
     <t xml:space="preserve">No open non-waived issues with both label Component:RTL and Type:Bug</t>
   </si>
   <si>
-    <t xml:space="preserve">Waiving can be done by applying the WAIVED:&lt;PROJECT_NAME&gt;. Issues labeled with a non-applicable parameter option are waived as well in case the RTL Freeze configuration applies to a different parameter configuration</t>
+    <t xml:space="preserve">Waiving can be done by applying the WAIVED:&lt;PROJECT_NAME&gt;. Issues labeled with a non-applicable parameter option are waived as well in case the release configuration applies to a different parameter configuration</t>
   </si>
   <si>
     <t xml:space="preserve">No dependency on external repositories for design</t>
@@ -762,7 +759,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84"/>
@@ -854,7 +851,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -870,10 +867,10 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1166,7 +1163,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1182,12 +1179,12 @@
   <dimension ref="B2:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1224,20 +1221,18 @@
       <c r="D3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="E3" s="10"/>
       <c r="F3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="124.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1245,10 +1240,10 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5"/>
       <c r="C5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -1256,36 +1251,36 @@
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5"/>
       <c r="C6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5"/>
       <c r="C7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -1293,36 +1288,36 @@
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
       <c r="C9" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5"/>
       <c r="C10" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="12" t="s">
         <v>65</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>66</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="9"/>
@@ -1330,10 +1325,10 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5"/>
       <c r="C12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -1341,23 +1336,23 @@
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5"/>
       <c r="C13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5"/>
       <c r="C14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -1365,10 +1360,10 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5"/>
       <c r="C15" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1376,36 +1371,36 @@
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5"/>
       <c r="C16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5"/>
       <c r="C17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="5"/>
       <c r="C18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -1413,10 +1408,10 @@
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="5"/>
       <c r="C19" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="9"/>
@@ -1424,23 +1419,23 @@
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5"/>
       <c r="C20" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5"/>
       <c r="C21" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1448,10 +1443,10 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5"/>
       <c r="C22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>90</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -1459,38 +1454,38 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5"/>
       <c r="C23" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="9"/>
@@ -1498,10 +1493,10 @@
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="14"/>
       <c r="C26" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -1509,10 +1504,10 @@
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="14"/>
       <c r="C27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -1520,10 +1515,10 @@
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="14"/>
       <c r="C28" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -1531,10 +1526,10 @@
     <row r="29" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="14"/>
       <c r="C29" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -1545,12 +1540,9 @@
     <mergeCell ref="B11:B23"/>
     <mergeCell ref="B25:B29"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="arjan.bink@silabs.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1569,7 +1561,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1598,161 +1590,161 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="17"/>
@@ -1761,7 +1753,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="17"/>
@@ -1770,7 +1762,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="17"/>
@@ -1786,7 +1778,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1802,10 +1794,10 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1834,105 +1826,105 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5"/>
       <c r="C6" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -1941,7 +1933,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
@@ -1950,7 +1942,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
@@ -1963,7 +1955,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1982,7 +1974,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -2015,7 +2007,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add IP worksheet (tab)
</commit_message>
<xml_diff>
--- a/process/OpenHW-Group-IP-Core-RTL-Freeze-Checklist-Templates/OpenHWGroup_TRL5_for_COREV_RTL_IP_Template.xlsx
+++ b/process/OpenHW-Group-IP-Core-RTL-Freeze-Checklist-Templates/OpenHWGroup_TRL5_for_COREV_RTL_IP_Template.xlsx
@@ -5,15 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Documentation" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="RTL Design" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Simulation Verification" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Formal Verification" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Software Requirements" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="IP" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="RTL Design" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Simulation Verification" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Formal Verification" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Software Requirements" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="153">
   <si>
     <t xml:space="preserve">Copyright 2020, 2023 by the OpenHW Group</t>
   </si>
@@ -154,6 +155,24 @@
   </si>
   <si>
     <t xml:space="preserve">Synthesis guidelines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP review of source code in RTL design repo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclipse “CQ” audit complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP review of source code in verification repo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP audit on User Manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenHW Staff audit compete</t>
   </si>
   <si>
     <t xml:space="preserve">Configuration</t>
@@ -322,9 +341,6 @@
   </si>
   <si>
     <t xml:space="preserve">Third-party audit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eclipse “CQ” audit complete</t>
   </si>
   <si>
     <t xml:space="preserve">No closed-source</t>
@@ -558,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -571,6 +587,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -599,7 +622,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -633,6 +656,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -755,11 +790,11 @@
   </sheetPr>
   <dimension ref="B2:B22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84"/>
@@ -870,7 +905,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1176,6 +1211,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="B2:F5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="51.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="51.13"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B5"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="B2:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1184,7 +1306,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1213,326 +1335,326 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="124.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5"/>
-      <c r="C5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="C5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5"/>
-      <c r="C6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
-        <v>53</v>
+      <c r="C6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5"/>
-      <c r="C7" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
-        <v>56</v>
+      <c r="C7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
-      <c r="C8" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="C8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
-      <c r="C9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>61</v>
+      <c r="C9" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5"/>
-      <c r="C10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
+      <c r="C10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5"/>
-      <c r="C12" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="C12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5"/>
-      <c r="C13" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9" t="s">
-        <v>70</v>
+      <c r="C13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5"/>
-      <c r="C14" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="C14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5"/>
-      <c r="C15" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="C15" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5"/>
-      <c r="C16" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
-        <v>75</v>
+      <c r="C16" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5"/>
-      <c r="C17" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9" t="s">
-        <v>78</v>
+      <c r="C17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="5"/>
-      <c r="C18" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="C18" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="5"/>
-      <c r="C19" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="9"/>
+      <c r="C19" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5"/>
-      <c r="C20" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9" t="s">
-        <v>85</v>
+      <c r="C20" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5"/>
-      <c r="C21" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="C21" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5"/>
-      <c r="C22" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="C22" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5"/>
-      <c r="C23" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9" t="s">
-        <v>92</v>
+      <c r="C23" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="9"/>
+        <v>99</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="9"/>
+      <c r="B25" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1550,7 +1672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1561,7 +1683,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1590,182 +1712,182 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="7" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="D10" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="15" t="n">
+        <v>133</v>
+      </c>
+      <c r="D11" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="7" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="17"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="17"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="7"/>
     </row>
   </sheetData>
@@ -1786,7 +1908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1797,7 +1919,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -1826,105 +1948,105 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5"/>
       <c r="C5" s="7" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5"/>
       <c r="C6" s="7" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5"/>
       <c r="C7" s="7" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="7" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="7" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -1933,7 +2055,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
@@ -1942,7 +2064,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
@@ -1963,7 +2085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1974,7 +2096,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -2002,7 +2124,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="18"/>
+      <c r="E3" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>